<commit_message>
internal Rmd file url ok
</commit_message>
<xml_diff>
--- a/content/course-econometrics/data/syllabus.xlsx
+++ b/content/course-econometrics/data/syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\netlify\content\course-econometrics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF29EDE-1296-42E9-8D3A-CD250C5998D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7B36F6-A09A-4873-8461-C9E92B3188A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="2010" windowWidth="25020" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>status_slide</t>
   </si>
@@ -292,6 +292,10 @@
   </si>
   <si>
     <t>第02章 一元回归：基本思想</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reading/cht01-history/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -620,7 +624,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -629,7 +633,7 @@
     <col min="2" max="2" width="9.375" customWidth="1"/>
     <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.625" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.625" customWidth="1"/>
     <col min="7" max="7" width="45.25" customWidth="1"/>
     <col min="8" max="8" width="90" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.75" customWidth="1"/>
@@ -720,7 +724,7 @@
         <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>

</xml_diff>